<commit_message>
Project Example 1 - Bank Rating is saved. Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
+++ b/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\OpenL\draft docs for mercurial\tut and examples with logo\org.openl.rules.demo.examples\Example 1 - Bank Rating\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4920" windowWidth="14895" windowHeight="3180" tabRatio="878"/>
+    <workbookView xWindow="-15" yWindow="4920" windowWidth="14895" windowHeight="3180" tabRatio="878" firstSheet="10" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Rating Algorithm" sheetId="18" r:id="rId1"/>
@@ -32,6 +27,7 @@
     <sheet name="Domain" sheetId="23" r:id="rId18"/>
     <sheet name="Vocabulary" sheetId="2" r:id="rId19"/>
     <sheet name="Test Data" sheetId="19" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="44" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="Deductible">Vocabulary!#REF!</definedName>
@@ -45,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="774">
   <si>
     <t>&gt; 51</t>
   </si>
@@ -4031,14 +4027,245 @@
   <si>
     <t>Datasets</t>
   </si>
+  <si>
+    <t>bank.bankID</t>
+  </si>
+  <si>
+    <t>bank.bankFullName</t>
+  </si>
+  <si>
+    <t>bank.countryCode</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.reportDate</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.totalAssets</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.claimsOnDemand</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.claimsUpTo3Months</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.claimsSecuredByPropertyCharges</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.claimsOnBanks</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.claimsOnCustomers</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.loanLossProvisionsForClaimsOnCustomers</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.otherAssets</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.capital</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.equity</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.liabilities</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.liabilitiesToBanks</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.liabilitiesToCustomers</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.liabilitiesOnDemand</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.liabilitiesToCustomersOnDemand</t>
+  </si>
+  <si>
+    <t>bank.currentFinancialData.consolidatedProfit</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.reportDate</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.totalAssets</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.claimsOnDemand</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.claimsUpTo3Months</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.claimsSecuredByPropertyCharges</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.claimsOnBanks</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.claimsOnCustomers</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.loanLossProvisionsForClaimsOnCustomers</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.otherAssets</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.capital</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.equity</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.liabilities</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.liabilitiesToBanks</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.liabilitiesToCustomers</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.liabilitiesOnDemand</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.liabilitiesToCustomersOnDemand</t>
+  </si>
+  <si>
+    <t>bank.previousFinancialData.consolidatedProfit</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.reportDate</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.lossesInThisYear</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.negativeHistoryRelations</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.negativeMassMedia</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.negativeInfoShareHoldersOrManagement</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.downgradesOfBankRating</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.isAdequateCoreCapitalRatio</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.isAdequateLiquidityRatio</t>
+  </si>
+  <si>
+    <t>bank.qualityIndicators.isAdequateMaxCreditRisk</t>
+  </si>
+  <si>
+    <t>bank.bankRatings.ratingAgency</t>
+  </si>
+  <si>
+    <t>bank.bankRatings.rating</t>
+  </si>
+  <si>
+    <t>754299</t>
+  </si>
+  <si>
+    <t>74502</t>
+  </si>
+  <si>
+    <t>179938</t>
+  </si>
+  <si>
+    <t>134321</t>
+  </si>
+  <si>
+    <t>110956</t>
+  </si>
+  <si>
+    <t>336872</t>
+  </si>
+  <si>
+    <t>9117</t>
+  </si>
+  <si>
+    <t>7349</t>
+  </si>
+  <si>
+    <t>40857</t>
+  </si>
+  <si>
+    <t>28658</t>
+  </si>
+  <si>
+    <t>725641</t>
+  </si>
+  <si>
+    <t>137626</t>
+  </si>
+  <si>
+    <t>262827</t>
+  </si>
+  <si>
+    <t>193986</t>
+  </si>
+  <si>
+    <t>143807</t>
+  </si>
+  <si>
+    <t>1489</t>
+  </si>
+  <si>
+    <t>69940</t>
+  </si>
+  <si>
+    <t>176674</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>41437</t>
+  </si>
+  <si>
+    <t>817527</t>
+  </si>
+  <si>
+    <t>264618</t>
+  </si>
+  <si>
+    <t>179283</t>
+  </si>
+  <si>
+    <t>-4633</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Bank inputs</t>
+  </si>
+  <si>
+    <t>Test BankRatingCalculation BankRatingTest1</t>
+  </si>
+  <si>
+    <t>The analysis of dynamic performance of such factors as capital (D1), quick liquidity (D2), liquidity (D3), profit (D4) and liabilities to customers (D5) is used for calculating the first correction index B1 (Balance Dynamic Index). Fe of B1 is the arithmetic mean of the scores of these five factors obtained: B1 = (D1 + D2 + D3 + D4 + D5) / 5.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -4128,7 +4355,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
@@ -4163,7 +4390,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="2" tint="-0.749992370372631"/>
+      <color theme="2" tint="-0.749992370372631" rgb="EEECE1"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
       <charset val="204"/>
@@ -4206,7 +4433,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4233,19 +4460,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
+        <fgColor theme="6" tint="-0.249977111117893" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4257,7 +4484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4269,13 +4496,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2" rgb="EEECE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4287,8 +4514,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -5386,7 +5623,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5397,7 +5634,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5410,7 +5647,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5835,10 +6072,10 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -6118,11 +6355,11 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -6135,7 +6372,7 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -6320,15 +6557,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="3"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6346,16 +6581,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -6431,7 +6666,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="5"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3"/>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6444,14 +6679,14 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="64" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6483,7 +6718,7 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="13" borderId="66" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="13" borderId="66" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="67" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6696,7 +6931,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="146" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="147" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="147" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="148" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="124" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6783,6 +7018,84 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="139" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="140" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="122" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="119" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="128" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="121" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="127" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="145" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="142" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6792,84 +7105,6 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="144" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="117" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="119" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="128" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="139" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="140" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="121" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="127" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="145" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="122" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6888,18 +7123,18 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="142" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="144" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="150" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6969,6 +7204,39 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="88" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="51" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="53" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="54" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6990,39 +7258,6 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="51" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="53" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="54" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7056,14 +7291,36 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Heading 1" xfId="5" builtinId="16"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 7" xfId="3"/>
     <cellStyle name="Normal_EPLI rater" xfId="1"/>
-    <cellStyle name="Обычный 2" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -7203,7 +7460,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7238,7 +7495,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7452,21 +7709,21 @@
   </sheetPr>
   <dimension ref="B1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="76.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="5.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" style="5" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="25.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="42.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="5" width="76.7109375" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="5" width="5.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="25.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="19.140625" collapsed="true"/>
+    <col min="12" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
@@ -7490,12 +7747,12 @@
     </row>
     <row r="4" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:10" ht="161.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="188" t="s">
+      <c r="D6" s="214" t="s">
         <v>537</v>
       </c>
-      <c r="E6" s="189"/>
-      <c r="F6" s="189"/>
-      <c r="G6" s="190"/>
+      <c r="E6" s="215"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="216"/>
     </row>
     <row r="7" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="152"/>
@@ -7504,12 +7761,12 @@
       <c r="G7" s="152"/>
     </row>
     <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="D9" s="204" t="s">
+      <c r="D9" s="188" t="s">
         <v>482</v>
       </c>
-      <c r="E9" s="205"/>
-      <c r="F9" s="205"/>
-      <c r="G9" s="206"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="190"/>
     </row>
     <row r="10" spans="2:10" ht="201" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="119" t="s">
@@ -7518,16 +7775,16 @@
       <c r="E10" s="120" t="s">
         <v>386</v>
       </c>
-      <c r="F10" s="197" t="s">
+      <c r="F10" s="194" t="s">
         <v>511</v>
       </c>
-      <c r="G10" s="198"/>
+      <c r="G10" s="195"/>
     </row>
     <row r="11" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="199" t="s">
+      <c r="D11" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="200"/>
+      <c r="E11" s="209"/>
       <c r="F11" s="127" t="s">
         <v>8</v>
       </c>
@@ -7537,11 +7794,11 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
-      <c r="D12" s="201" t="s">
+      <c r="D12" s="196" t="s">
         <v>608</v>
       </c>
-      <c r="E12" s="202"/>
-      <c r="F12" s="214"/>
+      <c r="E12" s="197"/>
+      <c r="F12" s="191"/>
       <c r="G12" s="118" t="s">
         <v>610</v>
       </c>
@@ -7551,32 +7808,32 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="16"/>
-      <c r="D13" s="193" t="s">
+      <c r="D13" s="198" t="s">
         <v>609</v>
       </c>
-      <c r="E13" s="194"/>
-      <c r="F13" s="215"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="192"/>
       <c r="G13" s="117" t="s">
         <v>611</v>
       </c>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D14" s="201" t="s">
+      <c r="D14" s="196" t="s">
         <v>182</v>
       </c>
-      <c r="E14" s="202"/>
+      <c r="E14" s="197"/>
       <c r="F14" s="123"/>
       <c r="G14" s="118" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D15" s="193" t="s">
+      <c r="D15" s="198" t="s">
         <v>179</v>
       </c>
-      <c r="E15" s="194"/>
-      <c r="F15" s="216" t="s">
+      <c r="E15" s="199"/>
+      <c r="F15" s="193" t="s">
         <v>612</v>
       </c>
       <c r="G15" s="117" t="s">
@@ -7584,30 +7841,30 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D16" s="193" t="s">
+      <c r="D16" s="198" t="s">
         <v>181</v>
       </c>
-      <c r="E16" s="194"/>
-      <c r="F16" s="216"/>
+      <c r="E16" s="199"/>
+      <c r="F16" s="193"/>
       <c r="G16" s="117" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="193" t="s">
+      <c r="D17" s="198" t="s">
         <v>183</v>
       </c>
-      <c r="E17" s="194"/>
-      <c r="F17" s="216"/>
+      <c r="E17" s="199"/>
+      <c r="F17" s="193"/>
       <c r="G17" s="117" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="60" x14ac:dyDescent="0.3">
-      <c r="D18" s="201" t="s">
+      <c r="D18" s="196" t="s">
         <v>180</v>
       </c>
-      <c r="E18" s="202"/>
+      <c r="E18" s="197"/>
       <c r="F18" s="160" t="s">
         <v>525</v>
       </c>
@@ -7617,10 +7874,10 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="16"/>
-      <c r="D19" s="193" t="s">
+      <c r="D19" s="198" t="s">
         <v>202</v>
       </c>
-      <c r="E19" s="194"/>
+      <c r="E19" s="199"/>
       <c r="F19" s="124" t="s">
         <v>193</v>
       </c>
@@ -7633,10 +7890,10 @@
     </row>
     <row r="20" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="52"/>
-      <c r="D20" s="210" t="s">
+      <c r="D20" s="204" t="s">
         <v>206</v>
       </c>
-      <c r="E20" s="211"/>
+      <c r="E20" s="205"/>
       <c r="F20" s="125" t="s">
         <v>513</v>
       </c>
@@ -7649,10 +7906,10 @@
     </row>
     <row r="21" spans="2:10" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="16"/>
-      <c r="D21" s="195" t="s">
+      <c r="D21" s="206" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="196"/>
+      <c r="E21" s="207"/>
       <c r="F21" s="126" t="s">
         <v>524</v>
       </c>
@@ -7665,12 +7922,12 @@
     </row>
     <row r="26" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B26" s="10"/>
-      <c r="D26" s="204" t="s">
+      <c r="D26" s="188" t="s">
         <v>648</v>
       </c>
-      <c r="E26" s="205"/>
-      <c r="F26" s="205"/>
-      <c r="G26" s="206"/>
+      <c r="E26" s="189"/>
+      <c r="F26" s="189"/>
+      <c r="G26" s="190"/>
       <c r="J26" s="10" t="s">
         <v>113</v>
       </c>
@@ -7683,19 +7940,19 @@
       <c r="E27" s="120" t="s">
         <v>386</v>
       </c>
-      <c r="F27" s="197" t="s">
+      <c r="F27" s="194" t="s">
         <v>492</v>
       </c>
-      <c r="G27" s="198" t="s">
+      <c r="G27" s="195" t="s">
         <v>393</v>
       </c>
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="199" t="s">
+      <c r="D28" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="200"/>
+      <c r="E28" s="209"/>
       <c r="F28" s="127" t="s">
         <v>8</v>
       </c>
@@ -7704,10 +7961,10 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D29" s="201" t="s">
+      <c r="D29" s="196" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="202"/>
+      <c r="E29" s="197"/>
       <c r="F29" s="124" t="s">
         <v>66</v>
       </c>
@@ -7716,10 +7973,10 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D30" s="191" t="s">
+      <c r="D30" s="202" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="192"/>
+      <c r="E30" s="203"/>
       <c r="F30" s="128" t="s">
         <v>514</v>
       </c>
@@ -7728,10 +7985,10 @@
       </c>
     </row>
     <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="D31" s="193" t="s">
+      <c r="D31" s="198" t="s">
         <v>363</v>
       </c>
-      <c r="E31" s="194"/>
+      <c r="E31" s="199"/>
       <c r="F31" s="124" t="s">
         <v>365</v>
       </c>
@@ -7740,10 +7997,10 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D32" s="191" t="s">
+      <c r="D32" s="202" t="s">
         <v>364</v>
       </c>
-      <c r="E32" s="192"/>
+      <c r="E32" s="203"/>
       <c r="F32" s="128" t="s">
         <v>517</v>
       </c>
@@ -7752,10 +8009,10 @@
       </c>
     </row>
     <row r="33" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="193" t="s">
+      <c r="D33" s="198" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="194"/>
+      <c r="E33" s="199"/>
       <c r="F33" s="124" t="s">
         <v>67</v>
       </c>
@@ -7764,10 +8021,10 @@
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D34" s="191" t="s">
+      <c r="D34" s="202" t="s">
         <v>185</v>
       </c>
-      <c r="E34" s="192"/>
+      <c r="E34" s="203"/>
       <c r="F34" s="128" t="s">
         <v>518</v>
       </c>
@@ -7776,10 +8033,10 @@
       </c>
     </row>
     <row r="35" spans="4:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="D35" s="193" t="s">
+      <c r="D35" s="198" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="194"/>
+      <c r="E35" s="199"/>
       <c r="F35" s="124" t="s">
         <v>68</v>
       </c>
@@ -7788,10 +8045,10 @@
       </c>
     </row>
     <row r="36" spans="4:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="D36" s="191" t="s">
+      <c r="D36" s="202" t="s">
         <v>186</v>
       </c>
-      <c r="E36" s="192"/>
+      <c r="E36" s="203"/>
       <c r="F36" s="128" t="s">
         <v>519</v>
       </c>
@@ -7800,10 +8057,10 @@
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="193" t="s">
+      <c r="D37" s="198" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="194"/>
+      <c r="E37" s="199"/>
       <c r="F37" s="124" t="s">
         <v>69</v>
       </c>
@@ -7812,10 +8069,10 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="191" t="s">
+      <c r="D38" s="202" t="s">
         <v>187</v>
       </c>
-      <c r="E38" s="192"/>
+      <c r="E38" s="203"/>
       <c r="F38" s="128" t="s">
         <v>520</v>
       </c>
@@ -7824,10 +8081,10 @@
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D39" s="193" t="s">
+      <c r="D39" s="198" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="194"/>
+      <c r="E39" s="199"/>
       <c r="F39" s="124" t="s">
         <v>70</v>
       </c>
@@ -7836,10 +8093,10 @@
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D40" s="191" t="s">
+      <c r="D40" s="202" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="192"/>
+      <c r="E40" s="203"/>
       <c r="F40" s="128" t="s">
         <v>521</v>
       </c>
@@ -7848,10 +8105,10 @@
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D41" s="193" t="s">
+      <c r="D41" s="198" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="194"/>
+      <c r="E41" s="199"/>
       <c r="F41" s="124" t="s">
         <v>71</v>
       </c>
@@ -7860,10 +8117,10 @@
       </c>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D42" s="191" t="s">
+      <c r="D42" s="202" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="192"/>
+      <c r="E42" s="203"/>
       <c r="F42" s="128" t="s">
         <v>522</v>
       </c>
@@ -7872,10 +8129,10 @@
       </c>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="193" t="s">
+      <c r="D43" s="198" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="194"/>
+      <c r="E43" s="199"/>
       <c r="F43" s="124" t="s">
         <v>72</v>
       </c>
@@ -7884,10 +8141,10 @@
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D44" s="191" t="s">
+      <c r="D44" s="202" t="s">
         <v>190</v>
       </c>
-      <c r="E44" s="192"/>
+      <c r="E44" s="203"/>
       <c r="F44" s="128" t="s">
         <v>523</v>
       </c>
@@ -7896,10 +8153,10 @@
       </c>
     </row>
     <row r="45" spans="4:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="D45" s="193" t="s">
+      <c r="D45" s="198" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="194"/>
+      <c r="E45" s="199"/>
       <c r="F45" s="124" t="s">
         <v>73</v>
       </c>
@@ -7908,10 +8165,10 @@
       </c>
     </row>
     <row r="46" spans="4:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="D46" s="191" t="s">
+      <c r="D46" s="202" t="s">
         <v>191</v>
       </c>
-      <c r="E46" s="192"/>
+      <c r="E46" s="203"/>
       <c r="F46" s="128" t="s">
         <v>516</v>
       </c>
@@ -7920,10 +8177,10 @@
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D47" s="193" t="s">
+      <c r="D47" s="198" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="194"/>
+      <c r="E47" s="199"/>
       <c r="F47" s="124" t="s">
         <v>74</v>
       </c>
@@ -7932,10 +8189,10 @@
       </c>
     </row>
     <row r="48" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D48" s="193" t="s">
+      <c r="D48" s="198" t="s">
         <v>192</v>
       </c>
-      <c r="E48" s="194"/>
+      <c r="E48" s="199"/>
       <c r="F48" s="124" t="s">
         <v>515</v>
       </c>
@@ -7944,10 +8201,10 @@
       </c>
     </row>
     <row r="49" spans="2:10" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D49" s="195" t="s">
+      <c r="D49" s="206" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="196"/>
+      <c r="E49" s="207"/>
       <c r="F49" s="161" t="s">
         <v>526</v>
       </c>
@@ -7963,12 +8220,12 @@
     </row>
     <row r="54" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B54" s="10"/>
-      <c r="D54" s="204" t="s">
+      <c r="D54" s="188" t="s">
         <v>615</v>
       </c>
-      <c r="E54" s="205"/>
-      <c r="F54" s="205"/>
-      <c r="G54" s="206"/>
+      <c r="E54" s="189"/>
+      <c r="F54" s="189"/>
+      <c r="G54" s="190"/>
       <c r="J54" s="10" t="s">
         <v>115</v>
       </c>
@@ -7981,19 +8238,19 @@
       <c r="E55" s="120" t="s">
         <v>386</v>
       </c>
-      <c r="F55" s="197" t="s">
-        <v>494</v>
-      </c>
-      <c r="G55" s="198" t="s">
+      <c r="F55" s="194" t="s">
+        <v>773</v>
+      </c>
+      <c r="G55" s="195" t="s">
         <v>393</v>
       </c>
       <c r="J55" s="10"/>
     </row>
     <row r="56" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D56" s="199" t="s">
+      <c r="D56" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="E56" s="200"/>
+      <c r="E56" s="209"/>
       <c r="F56" s="127" t="s">
         <v>8</v>
       </c>
@@ -8002,10 +8259,10 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D57" s="201" t="s">
+      <c r="D57" s="196" t="s">
         <v>116</v>
       </c>
-      <c r="E57" s="202"/>
+      <c r="E57" s="197"/>
       <c r="F57" s="124" t="s">
         <v>118</v>
       </c>
@@ -8014,10 +8271,10 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="191" t="s">
+      <c r="D58" s="202" t="s">
         <v>117</v>
       </c>
-      <c r="E58" s="192"/>
+      <c r="E58" s="203"/>
       <c r="F58" s="128" t="s">
         <v>527</v>
       </c>
@@ -8026,10 +8283,10 @@
       </c>
     </row>
     <row r="59" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="193" t="s">
+      <c r="D59" s="198" t="s">
         <v>133</v>
       </c>
-      <c r="E59" s="194"/>
+      <c r="E59" s="199"/>
       <c r="F59" s="124" t="s">
         <v>135</v>
       </c>
@@ -8038,10 +8295,10 @@
       </c>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="191" t="s">
+      <c r="D60" s="202" t="s">
         <v>134</v>
       </c>
-      <c r="E60" s="192"/>
+      <c r="E60" s="203"/>
       <c r="F60" s="128" t="s">
         <v>528</v>
       </c>
@@ -8050,10 +8307,10 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="D61" s="193" t="s">
+      <c r="D61" s="198" t="s">
         <v>131</v>
       </c>
-      <c r="E61" s="194"/>
+      <c r="E61" s="199"/>
       <c r="F61" s="124" t="s">
         <v>136</v>
       </c>
@@ -8062,10 +8319,10 @@
       </c>
     </row>
     <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="191" t="s">
+      <c r="D62" s="202" t="s">
         <v>132</v>
       </c>
-      <c r="E62" s="192"/>
+      <c r="E62" s="203"/>
       <c r="F62" s="128" t="s">
         <v>529</v>
       </c>
@@ -8074,10 +8331,10 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="193" t="s">
+      <c r="D63" s="198" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="194"/>
+      <c r="E63" s="199"/>
       <c r="F63" s="124" t="s">
         <v>141</v>
       </c>
@@ -8086,10 +8343,10 @@
       </c>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="191" t="s">
+      <c r="D64" s="202" t="s">
         <v>138</v>
       </c>
-      <c r="E64" s="192"/>
+      <c r="E64" s="203"/>
       <c r="F64" s="128" t="s">
         <v>530</v>
       </c>
@@ -8098,10 +8355,10 @@
       </c>
     </row>
     <row r="65" spans="2:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="D65" s="193" t="s">
+      <c r="D65" s="198" t="s">
         <v>142</v>
       </c>
-      <c r="E65" s="194"/>
+      <c r="E65" s="199"/>
       <c r="F65" s="124" t="s">
         <v>144</v>
       </c>
@@ -8110,10 +8367,10 @@
       </c>
     </row>
     <row r="66" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="191" t="s">
+      <c r="D66" s="202" t="s">
         <v>143</v>
       </c>
-      <c r="E66" s="192"/>
+      <c r="E66" s="203"/>
       <c r="F66" s="128" t="s">
         <v>531</v>
       </c>
@@ -8122,10 +8379,10 @@
       </c>
     </row>
     <row r="67" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D67" s="193" t="s">
+      <c r="D67" s="198" t="s">
         <v>145</v>
       </c>
-      <c r="E67" s="194"/>
+      <c r="E67" s="199"/>
       <c r="F67" s="151" t="s">
         <v>532</v>
       </c>
@@ -8134,10 +8391,10 @@
       </c>
     </row>
     <row r="68" spans="2:10" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D68" s="195" t="s">
+      <c r="D68" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="E68" s="196"/>
+      <c r="E68" s="207"/>
       <c r="F68" s="126"/>
       <c r="G68" s="122" t="s">
         <v>420</v>
@@ -8145,12 +8402,12 @@
     </row>
     <row r="73" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B73" s="16"/>
-      <c r="D73" s="204" t="s">
+      <c r="D73" s="188" t="s">
         <v>483</v>
       </c>
-      <c r="E73" s="205"/>
-      <c r="F73" s="205"/>
-      <c r="G73" s="206"/>
+      <c r="E73" s="189"/>
+      <c r="F73" s="189"/>
+      <c r="G73" s="190"/>
       <c r="J73" s="16" t="s">
         <v>169</v>
       </c>
@@ -8163,19 +8420,19 @@
       <c r="E74" s="120" t="s">
         <v>386</v>
       </c>
-      <c r="F74" s="197" t="s">
+      <c r="F74" s="194" t="s">
         <v>495</v>
       </c>
-      <c r="G74" s="198" t="s">
+      <c r="G74" s="195" t="s">
         <v>393</v>
       </c>
       <c r="J74" s="16"/>
     </row>
     <row r="75" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D75" s="199" t="s">
+      <c r="D75" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="200"/>
+      <c r="E75" s="209"/>
       <c r="F75" s="127" t="s">
         <v>8</v>
       </c>
@@ -8184,11 +8441,11 @@
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D76" s="201" t="s">
+      <c r="D76" s="196" t="s">
         <v>152</v>
       </c>
-      <c r="E76" s="202"/>
-      <c r="F76" s="207" t="s">
+      <c r="E76" s="197"/>
+      <c r="F76" s="211" t="s">
         <v>533</v>
       </c>
       <c r="G76" s="117" t="s">
@@ -8196,60 +8453,60 @@
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D77" s="193" t="s">
+      <c r="D77" s="198" t="s">
         <v>153</v>
       </c>
-      <c r="E77" s="203"/>
-      <c r="F77" s="208"/>
+      <c r="E77" s="210"/>
+      <c r="F77" s="212"/>
       <c r="G77" s="155" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D78" s="193" t="s">
+      <c r="D78" s="198" t="s">
         <v>154</v>
       </c>
-      <c r="E78" s="194"/>
-      <c r="F78" s="208"/>
+      <c r="E78" s="199"/>
+      <c r="F78" s="212"/>
       <c r="G78" s="117" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="79" spans="2:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="D79" s="193" t="s">
+      <c r="D79" s="198" t="s">
         <v>155</v>
       </c>
-      <c r="E79" s="203"/>
-      <c r="F79" s="208"/>
+      <c r="E79" s="210"/>
+      <c r="F79" s="212"/>
       <c r="G79" s="155" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D80" s="193" t="s">
+      <c r="D80" s="198" t="s">
         <v>156</v>
       </c>
-      <c r="E80" s="194"/>
-      <c r="F80" s="208"/>
+      <c r="E80" s="199"/>
+      <c r="F80" s="212"/>
       <c r="G80" s="117" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D81" s="191" t="s">
+      <c r="D81" s="202" t="s">
         <v>165</v>
       </c>
-      <c r="E81" s="192"/>
-      <c r="F81" s="209"/>
+      <c r="E81" s="203"/>
+      <c r="F81" s="213"/>
       <c r="G81" s="129" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="82" spans="2:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D82" s="193" t="s">
+      <c r="D82" s="198" t="s">
         <v>177</v>
       </c>
-      <c r="E82" s="194"/>
+      <c r="E82" s="199"/>
       <c r="F82" s="124" t="s">
         <v>534</v>
       </c>
@@ -8258,10 +8515,10 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D83" s="195" t="s">
+      <c r="D83" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="E83" s="196"/>
+      <c r="E83" s="207"/>
       <c r="F83" s="126"/>
       <c r="G83" s="122" t="s">
         <v>427</v>
@@ -8269,12 +8526,12 @@
     </row>
     <row r="88" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B88" s="16"/>
-      <c r="D88" s="204" t="s">
+      <c r="D88" s="188" t="s">
         <v>484</v>
       </c>
-      <c r="E88" s="205"/>
-      <c r="F88" s="205"/>
-      <c r="G88" s="206"/>
+      <c r="E88" s="189"/>
+      <c r="F88" s="189"/>
+      <c r="G88" s="190"/>
       <c r="J88" s="16" t="s">
         <v>207</v>
       </c>
@@ -8287,19 +8544,19 @@
       <c r="E89" s="120" t="s">
         <v>386</v>
       </c>
-      <c r="F89" s="197" t="s">
+      <c r="F89" s="194" t="s">
         <v>496</v>
       </c>
-      <c r="G89" s="198" t="s">
+      <c r="G89" s="195" t="s">
         <v>393</v>
       </c>
       <c r="J89" s="16"/>
     </row>
     <row r="90" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D90" s="199" t="s">
+      <c r="D90" s="208" t="s">
         <v>7</v>
       </c>
-      <c r="E90" s="200"/>
+      <c r="E90" s="209"/>
       <c r="F90" s="127" t="s">
         <v>8</v>
       </c>
@@ -8308,11 +8565,11 @@
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D91" s="201" t="s">
+      <c r="D91" s="196" t="s">
         <v>173</v>
       </c>
-      <c r="E91" s="202"/>
-      <c r="F91" s="212" t="s">
+      <c r="E91" s="197"/>
+      <c r="F91" s="200" t="s">
         <v>535</v>
       </c>
       <c r="G91" s="117" t="s">
@@ -8320,40 +8577,40 @@
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D92" s="193" t="s">
+      <c r="D92" s="198" t="s">
         <v>175</v>
       </c>
-      <c r="E92" s="203"/>
-      <c r="F92" s="213"/>
+      <c r="E92" s="210"/>
+      <c r="F92" s="201"/>
       <c r="G92" s="155" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="D93" s="193" t="s">
+      <c r="D93" s="198" t="s">
         <v>174</v>
       </c>
-      <c r="E93" s="194"/>
-      <c r="F93" s="213"/>
+      <c r="E93" s="199"/>
+      <c r="F93" s="201"/>
       <c r="G93" s="117" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D94" s="191" t="s">
+      <c r="D94" s="202" t="s">
         <v>176</v>
       </c>
-      <c r="E94" s="192"/>
-      <c r="F94" s="213"/>
+      <c r="E94" s="203"/>
+      <c r="F94" s="201"/>
       <c r="G94" s="129" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="95" spans="2:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D95" s="193" t="s">
+      <c r="D95" s="198" t="s">
         <v>178</v>
       </c>
-      <c r="E95" s="194"/>
+      <c r="E95" s="199"/>
       <c r="F95" s="125" t="s">
         <v>536</v>
       </c>
@@ -8362,10 +8619,10 @@
       </c>
     </row>
     <row r="96" spans="2:10" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D96" s="195" t="s">
+      <c r="D96" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="E96" s="196"/>
+      <c r="E96" s="207"/>
       <c r="F96" s="126"/>
       <c r="G96" s="122" t="s">
         <v>432</v>
@@ -8373,16 +8630,57 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="F76:F81"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D88:G88"/>
     <mergeCell ref="F91:F94"/>
     <mergeCell ref="D29:E29"/>
@@ -8399,57 +8697,16 @@
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="F76:F81"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J26" location="'Balance Quality'!A1" display="'Balance Quality'!A1"/>
@@ -8476,9 +8733,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -8661,9 +8918,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -8690,11 +8947,11 @@
     </row>
     <row r="5" spans="1:6" s="15" customFormat="1" ht="219" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
-      <c r="C5" s="188" t="s">
+      <c r="C5" s="214" t="s">
         <v>567</v>
       </c>
-      <c r="D5" s="189"/>
-      <c r="E5" s="190"/>
+      <c r="D5" s="215"/>
+      <c r="E5" s="216"/>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -8703,10 +8960,10 @@
       <c r="F6" s="16"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="225" t="s">
+      <c r="C8" s="223" t="s">
         <v>670</v>
       </c>
-      <c r="D8" s="225"/>
+      <c r="D8" s="223"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="39" t="s">
@@ -8792,8 +9049,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -8898,18 +9155,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="4.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="3.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -8936,7 +9193,7 @@
     </row>
     <row r="5" spans="1:15" s="15" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
-      <c r="D5" s="188" t="s">
+      <c r="D5" s="214" t="s">
         <v>568</v>
       </c>
       <c r="E5" s="244"/>
@@ -8947,28 +9204,28 @@
       <c r="O6" s="16"/>
     </row>
     <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="C8" s="204" t="s">
+      <c r="C8" s="188" t="s">
         <v>481</v>
       </c>
-      <c r="D8" s="205"/>
-      <c r="E8" s="205"/>
-      <c r="F8" s="205"/>
-      <c r="G8" s="205"/>
-      <c r="H8" s="205"/>
-      <c r="I8" s="205"/>
-      <c r="J8" s="205"/>
-      <c r="K8" s="205"/>
-      <c r="L8" s="205"/>
-      <c r="M8" s="206"/>
+      <c r="D8" s="189"/>
+      <c r="E8" s="189"/>
+      <c r="F8" s="189"/>
+      <c r="G8" s="189"/>
+      <c r="H8" s="189"/>
+      <c r="I8" s="189"/>
+      <c r="J8" s="189"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="189"/>
+      <c r="M8" s="190"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C9" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="250" t="s">
+      <c r="D9" s="261" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="251"/>
+      <c r="E9" s="262"/>
       <c r="F9" s="116" t="s">
         <v>124</v>
       </c>
@@ -8988,10 +9245,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C10" s="90"/>
-      <c r="D10" s="252" t="s">
+      <c r="D10" s="263" t="s">
         <v>234</v>
       </c>
-      <c r="E10" s="253"/>
+      <c r="E10" s="264"/>
       <c r="F10" s="102" t="s">
         <v>467</v>
       </c>
@@ -9031,35 +9288,35 @@
       <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:15" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="263" t="s">
+      <c r="C12" s="256" t="s">
         <v>450</v>
       </c>
-      <c r="D12" s="254" t="s">
+      <c r="D12" s="265" t="s">
         <v>213</v>
       </c>
-      <c r="E12" s="254" t="s">
+      <c r="E12" s="265" t="s">
         <v>212</v>
       </c>
-      <c r="F12" s="256" t="s">
+      <c r="F12" s="267" t="s">
         <v>603</v>
       </c>
-      <c r="G12" s="257" t="s">
+      <c r="G12" s="250" t="s">
         <v>566</v>
       </c>
-      <c r="H12" s="258"/>
-      <c r="I12" s="258"/>
-      <c r="J12" s="258" t="s">
+      <c r="H12" s="251"/>
+      <c r="I12" s="251"/>
+      <c r="J12" s="251" t="s">
         <v>230</v>
       </c>
-      <c r="K12" s="258"/>
-      <c r="L12" s="258"/>
+      <c r="K12" s="251"/>
+      <c r="L12" s="251"/>
       <c r="M12" s="96"/>
     </row>
     <row r="13" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="264"/>
-      <c r="D13" s="255"/>
-      <c r="E13" s="255"/>
-      <c r="F13" s="255"/>
+      <c r="C13" s="257"/>
+      <c r="D13" s="266"/>
+      <c r="E13" s="266"/>
+      <c r="F13" s="266"/>
       <c r="G13" s="26" t="s">
         <v>538</v>
       </c>
@@ -9091,15 +9348,15 @@
         <v>334</v>
       </c>
       <c r="F14" s="231"/>
-      <c r="G14" s="259">
+      <c r="G14" s="252">
         <v>1</v>
       </c>
-      <c r="H14" s="259"/>
-      <c r="I14" s="259"/>
-      <c r="J14" s="259"/>
-      <c r="K14" s="259"/>
-      <c r="L14" s="259"/>
-      <c r="M14" s="260"/>
+      <c r="H14" s="252"/>
+      <c r="I14" s="252"/>
+      <c r="J14" s="252"/>
+      <c r="K14" s="252"/>
+      <c r="L14" s="252"/>
+      <c r="M14" s="253"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C15" s="33">
@@ -9112,13 +9369,13 @@
         <v>335</v>
       </c>
       <c r="F15" s="232"/>
-      <c r="G15" s="259"/>
-      <c r="H15" s="259"/>
-      <c r="I15" s="259"/>
-      <c r="J15" s="259"/>
-      <c r="K15" s="259"/>
-      <c r="L15" s="259"/>
-      <c r="M15" s="260"/>
+      <c r="G15" s="252"/>
+      <c r="H15" s="252"/>
+      <c r="I15" s="252"/>
+      <c r="J15" s="252"/>
+      <c r="K15" s="252"/>
+      <c r="L15" s="252"/>
+      <c r="M15" s="253"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C16" s="33">
@@ -9131,13 +9388,13 @@
         <v>335</v>
       </c>
       <c r="F16" s="233"/>
-      <c r="G16" s="259"/>
-      <c r="H16" s="259"/>
-      <c r="I16" s="259"/>
-      <c r="J16" s="259"/>
-      <c r="K16" s="259"/>
-      <c r="L16" s="259"/>
-      <c r="M16" s="260"/>
+      <c r="G16" s="252"/>
+      <c r="H16" s="252"/>
+      <c r="I16" s="252"/>
+      <c r="J16" s="252"/>
+      <c r="K16" s="252"/>
+      <c r="L16" s="252"/>
+      <c r="M16" s="253"/>
     </row>
     <row r="17" spans="3:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C17" s="33">
@@ -9149,18 +9406,18 @@
       <c r="E17" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="F17" s="265" t="s">
+      <c r="F17" s="258" t="s">
         <v>236</v>
       </c>
-      <c r="G17" s="259">
+      <c r="G17" s="252">
         <v>0.8</v>
       </c>
-      <c r="H17" s="259"/>
-      <c r="I17" s="259"/>
-      <c r="J17" s="259"/>
-      <c r="K17" s="259"/>
-      <c r="L17" s="259"/>
-      <c r="M17" s="260"/>
+      <c r="H17" s="252"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="252"/>
+      <c r="K17" s="252"/>
+      <c r="L17" s="252"/>
+      <c r="M17" s="253"/>
     </row>
     <row r="18" spans="3:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="33">
@@ -9173,13 +9430,13 @@
         <v>337</v>
       </c>
       <c r="F18" s="232"/>
-      <c r="G18" s="259"/>
-      <c r="H18" s="259"/>
-      <c r="I18" s="259"/>
-      <c r="J18" s="259"/>
-      <c r="K18" s="259"/>
-      <c r="L18" s="259"/>
-      <c r="M18" s="260"/>
+      <c r="G18" s="252"/>
+      <c r="H18" s="252"/>
+      <c r="I18" s="252"/>
+      <c r="J18" s="252"/>
+      <c r="K18" s="252"/>
+      <c r="L18" s="252"/>
+      <c r="M18" s="253"/>
     </row>
     <row r="19" spans="3:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="33">
@@ -9192,20 +9449,20 @@
         <v>337</v>
       </c>
       <c r="F19" s="233"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="259"/>
-      <c r="I19" s="259"/>
-      <c r="J19" s="259"/>
-      <c r="K19" s="259"/>
-      <c r="L19" s="259"/>
-      <c r="M19" s="260"/>
+      <c r="G19" s="252"/>
+      <c r="H19" s="252"/>
+      <c r="I19" s="252"/>
+      <c r="J19" s="252"/>
+      <c r="K19" s="252"/>
+      <c r="L19" s="252"/>
+      <c r="M19" s="253"/>
     </row>
     <row r="20" spans="3:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="33">
         <v>7</v>
       </c>
-      <c r="D20" s="265"/>
-      <c r="E20" s="265"/>
+      <c r="D20" s="258"/>
+      <c r="E20" s="258"/>
       <c r="F20" s="21" t="s">
         <v>194</v>
       </c>
@@ -9328,20 +9585,20 @@
       <c r="C24" s="35">
         <v>11</v>
       </c>
-      <c r="D24" s="266"/>
-      <c r="E24" s="267"/>
+      <c r="D24" s="259"/>
+      <c r="E24" s="260"/>
       <c r="F24" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="261">
+      <c r="G24" s="254">
         <v>0</v>
       </c>
-      <c r="H24" s="261"/>
-      <c r="I24" s="261"/>
-      <c r="J24" s="261"/>
-      <c r="K24" s="261"/>
-      <c r="L24" s="261"/>
-      <c r="M24" s="262"/>
+      <c r="H24" s="254"/>
+      <c r="I24" s="254"/>
+      <c r="J24" s="254"/>
+      <c r="K24" s="254"/>
+      <c r="L24" s="254"/>
+      <c r="M24" s="255"/>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D29" s="237"/>
@@ -9386,6 +9643,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="C8:M8"/>
@@ -9396,14 +9661,6 @@
     <mergeCell ref="G17:M19"/>
     <mergeCell ref="D20:D24"/>
     <mergeCell ref="E20:E24"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O1" location="'Rating Algorithm'!A20" display="Rating Algorithm'!A20"/>
@@ -9421,9 +9678,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -9508,9 +9765,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2" collapsed="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="35.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
@@ -9529,10 +9786,10 @@
       <c r="F3" s="16"/>
     </row>
     <row r="4" spans="2:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="188" t="s">
+      <c r="C4" s="214" t="s">
         <v>508</v>
       </c>
-      <c r="D4" s="190"/>
+      <c r="D4" s="216"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -9582,10 +9839,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="48.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="48.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
@@ -9878,8 +10135,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -9963,10 +10220,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="39.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -10390,10 +10647,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="2" collapsed="1"/>
-    <col min="4" max="4" width="34.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="3" style="2" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="34.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="30.0" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -11256,13 +11513,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -11532,27 +11791,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="48.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="3.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="51.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="30.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="32.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="48.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="25.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="23.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="21" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -12051,6 +12310,544 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:AY8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:AW5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:51" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="4" spans="2:51" s="15" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="279" t="s">
+        <v>697</v>
+      </c>
+      <c r="C4" s="279" t="s">
+        <v>698</v>
+      </c>
+      <c r="D4" s="279" t="s">
+        <v>699</v>
+      </c>
+      <c r="E4" s="279" t="s">
+        <v>700</v>
+      </c>
+      <c r="F4" s="279" t="s">
+        <v>701</v>
+      </c>
+      <c r="G4" s="279" t="s">
+        <v>702</v>
+      </c>
+      <c r="H4" s="279" t="s">
+        <v>703</v>
+      </c>
+      <c r="I4" s="279" t="s">
+        <v>704</v>
+      </c>
+      <c r="J4" s="279" t="s">
+        <v>705</v>
+      </c>
+      <c r="K4" s="279" t="s">
+        <v>706</v>
+      </c>
+      <c r="L4" s="279" t="s">
+        <v>707</v>
+      </c>
+      <c r="M4" s="279" t="s">
+        <v>708</v>
+      </c>
+      <c r="N4" s="279" t="s">
+        <v>709</v>
+      </c>
+      <c r="O4" s="279" t="s">
+        <v>710</v>
+      </c>
+      <c r="P4" s="279" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q4" s="279" t="s">
+        <v>712</v>
+      </c>
+      <c r="R4" s="279" t="s">
+        <v>713</v>
+      </c>
+      <c r="S4" s="279" t="s">
+        <v>714</v>
+      </c>
+      <c r="T4" s="279" t="s">
+        <v>715</v>
+      </c>
+      <c r="U4" s="279" t="s">
+        <v>716</v>
+      </c>
+      <c r="V4" s="279" t="s">
+        <v>717</v>
+      </c>
+      <c r="W4" s="279" t="s">
+        <v>718</v>
+      </c>
+      <c r="X4" s="279" t="s">
+        <v>719</v>
+      </c>
+      <c r="Y4" s="279" t="s">
+        <v>720</v>
+      </c>
+      <c r="Z4" s="279" t="s">
+        <v>721</v>
+      </c>
+      <c r="AA4" s="279" t="s">
+        <v>722</v>
+      </c>
+      <c r="AB4" s="279" t="s">
+        <v>723</v>
+      </c>
+      <c r="AC4" s="279" t="s">
+        <v>724</v>
+      </c>
+      <c r="AD4" s="279" t="s">
+        <v>725</v>
+      </c>
+      <c r="AE4" s="279" t="s">
+        <v>726</v>
+      </c>
+      <c r="AF4" s="279" t="s">
+        <v>727</v>
+      </c>
+      <c r="AG4" s="279" t="s">
+        <v>728</v>
+      </c>
+      <c r="AH4" s="279" t="s">
+        <v>729</v>
+      </c>
+      <c r="AI4" s="279" t="s">
+        <v>730</v>
+      </c>
+      <c r="AJ4" s="279" t="s">
+        <v>731</v>
+      </c>
+      <c r="AK4" s="279" t="s">
+        <v>732</v>
+      </c>
+      <c r="AL4" s="279" t="s">
+        <v>733</v>
+      </c>
+      <c r="AM4" s="279" t="s">
+        <v>734</v>
+      </c>
+      <c r="AN4" s="279" t="s">
+        <v>735</v>
+      </c>
+      <c r="AO4" s="279" t="s">
+        <v>736</v>
+      </c>
+      <c r="AP4" s="279" t="s">
+        <v>737</v>
+      </c>
+      <c r="AQ4" s="279" t="s">
+        <v>738</v>
+      </c>
+      <c r="AR4" s="279" t="s">
+        <v>739</v>
+      </c>
+      <c r="AS4" s="279" t="s">
+        <v>740</v>
+      </c>
+      <c r="AT4" s="279" t="s">
+        <v>741</v>
+      </c>
+      <c r="AU4" s="279" t="s">
+        <v>742</v>
+      </c>
+      <c r="AV4" s="279" t="s">
+        <v>743</v>
+      </c>
+      <c r="AW4" s="279" t="s">
+        <v>744</v>
+      </c>
+      <c r="AX4" s="131" t="s">
+        <v>203</v>
+      </c>
+      <c r="AY4" s="132" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="2:51" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="284" t="s">
+        <v>771</v>
+      </c>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285"/>
+      <c r="H5" s="285"/>
+      <c r="I5" s="285"/>
+      <c r="J5" s="285"/>
+      <c r="K5" s="285"/>
+      <c r="L5" s="285"/>
+      <c r="M5" s="285"/>
+      <c r="N5" s="285"/>
+      <c r="O5" s="285"/>
+      <c r="P5" s="285"/>
+      <c r="Q5" s="285"/>
+      <c r="R5" s="285"/>
+      <c r="S5" s="285"/>
+      <c r="T5" s="285"/>
+      <c r="U5" s="285"/>
+      <c r="V5" s="285"/>
+      <c r="W5" s="285"/>
+      <c r="X5" s="285"/>
+      <c r="Y5" s="285"/>
+      <c r="Z5" s="285"/>
+      <c r="AA5" s="285"/>
+      <c r="AB5" s="285"/>
+      <c r="AC5" s="285"/>
+      <c r="AD5" s="285"/>
+      <c r="AE5" s="285"/>
+      <c r="AF5" s="285"/>
+      <c r="AG5" s="285"/>
+      <c r="AH5" s="285"/>
+      <c r="AI5" s="285"/>
+      <c r="AJ5" s="285"/>
+      <c r="AK5" s="285"/>
+      <c r="AL5" s="285"/>
+      <c r="AM5" s="285"/>
+      <c r="AN5" s="285"/>
+      <c r="AO5" s="285"/>
+      <c r="AP5" s="285"/>
+      <c r="AQ5" s="285"/>
+      <c r="AR5" s="285"/>
+      <c r="AS5" s="285"/>
+      <c r="AT5" s="285"/>
+      <c r="AU5" s="285"/>
+      <c r="AV5" s="285"/>
+      <c r="AW5" s="286"/>
+      <c r="AX5" s="139" t="s">
+        <v>201</v>
+      </c>
+      <c r="AY5" s="140" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="2:51" s="15" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="280" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="280" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="280" t="s">
+        <v>550</v>
+      </c>
+      <c r="E6" s="281">
+        <v>40179</v>
+      </c>
+      <c r="F6" s="280" t="s">
+        <v>745</v>
+      </c>
+      <c r="G6" s="280" t="s">
+        <v>746</v>
+      </c>
+      <c r="H6" s="280" t="s">
+        <v>747</v>
+      </c>
+      <c r="I6" s="280" t="s">
+        <v>748</v>
+      </c>
+      <c r="J6" s="280" t="s">
+        <v>749</v>
+      </c>
+      <c r="K6" s="280" t="s">
+        <v>750</v>
+      </c>
+      <c r="L6" s="280" t="s">
+        <v>751</v>
+      </c>
+      <c r="M6" s="280" t="s">
+        <v>752</v>
+      </c>
+      <c r="N6" s="280" t="s">
+        <v>753</v>
+      </c>
+      <c r="O6" s="280" t="s">
+        <v>754</v>
+      </c>
+      <c r="P6" s="280" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q6" s="280" t="s">
+        <v>756</v>
+      </c>
+      <c r="R6" s="280" t="s">
+        <v>757</v>
+      </c>
+      <c r="S6" s="280" t="s">
+        <v>758</v>
+      </c>
+      <c r="T6" s="280" t="s">
+        <v>759</v>
+      </c>
+      <c r="U6" s="280" t="s">
+        <v>760</v>
+      </c>
+      <c r="V6" s="281">
+        <v>39814</v>
+      </c>
+      <c r="W6" s="280" t="s">
+        <v>590</v>
+      </c>
+      <c r="X6" s="280" t="s">
+        <v>761</v>
+      </c>
+      <c r="Y6" s="280" t="s">
+        <v>762</v>
+      </c>
+      <c r="Z6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AA6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AB6" s="280" t="s">
+        <v>590</v>
+      </c>
+      <c r="AC6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AD6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AE6" s="280" t="s">
+        <v>764</v>
+      </c>
+      <c r="AF6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AG6" s="280" t="s">
+        <v>765</v>
+      </c>
+      <c r="AH6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AI6" s="280" t="s">
+        <v>766</v>
+      </c>
+      <c r="AJ6" s="280" t="s">
+        <v>767</v>
+      </c>
+      <c r="AK6" s="280" t="s">
+        <v>763</v>
+      </c>
+      <c r="AL6" s="280" t="s">
+        <v>768</v>
+      </c>
+      <c r="AM6" s="281">
+        <v>40179</v>
+      </c>
+      <c r="AN6" s="280" t="s">
+        <v>769</v>
+      </c>
+      <c r="AO6" s="280" t="s">
+        <v>769</v>
+      </c>
+      <c r="AP6" s="280" t="s">
+        <v>769</v>
+      </c>
+      <c r="AQ6" s="280" t="s">
+        <v>769</v>
+      </c>
+      <c r="AR6" s="280" t="s">
+        <v>770</v>
+      </c>
+      <c r="AS6" s="280" t="s">
+        <v>770</v>
+      </c>
+      <c r="AT6" s="280" t="s">
+        <v>770</v>
+      </c>
+      <c r="AU6" s="280" t="s">
+        <v>770</v>
+      </c>
+      <c r="AV6" s="282" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW6" s="282" t="s">
+        <v>220</v>
+      </c>
+      <c r="AX6" s="142" t="s">
+        <v>196</v>
+      </c>
+      <c r="AY6" s="143">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:51" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="283"/>
+      <c r="C7" s="283"/>
+      <c r="D7" s="283"/>
+      <c r="E7" s="283"/>
+      <c r="F7" s="283"/>
+      <c r="G7" s="283"/>
+      <c r="H7" s="283"/>
+      <c r="I7" s="283"/>
+      <c r="J7" s="283"/>
+      <c r="K7" s="283"/>
+      <c r="L7" s="283"/>
+      <c r="M7" s="283"/>
+      <c r="N7" s="283"/>
+      <c r="O7" s="283"/>
+      <c r="P7" s="283"/>
+      <c r="Q7" s="283"/>
+      <c r="R7" s="283"/>
+      <c r="S7" s="283"/>
+      <c r="T7" s="283"/>
+      <c r="U7" s="283"/>
+      <c r="V7" s="283"/>
+      <c r="W7" s="283"/>
+      <c r="X7" s="283"/>
+      <c r="Y7" s="283"/>
+      <c r="Z7" s="283"/>
+      <c r="AA7" s="283"/>
+      <c r="AB7" s="283"/>
+      <c r="AC7" s="283"/>
+      <c r="AD7" s="283"/>
+      <c r="AE7" s="283"/>
+      <c r="AF7" s="283"/>
+      <c r="AG7" s="283"/>
+      <c r="AH7" s="283"/>
+      <c r="AI7" s="283"/>
+      <c r="AJ7" s="283"/>
+      <c r="AK7" s="283"/>
+      <c r="AL7" s="283"/>
+      <c r="AM7" s="283"/>
+      <c r="AN7" s="283"/>
+      <c r="AO7" s="283"/>
+      <c r="AP7" s="283"/>
+      <c r="AQ7" s="283"/>
+      <c r="AR7" s="283"/>
+      <c r="AS7" s="283"/>
+      <c r="AT7" s="283"/>
+      <c r="AU7" s="283"/>
+      <c r="AV7" s="282" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW7" s="282" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="2:51" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="B8" s="283"/>
+      <c r="C8" s="283"/>
+      <c r="D8" s="283"/>
+      <c r="E8" s="283"/>
+      <c r="F8" s="283"/>
+      <c r="G8" s="283"/>
+      <c r="H8" s="283"/>
+      <c r="I8" s="283"/>
+      <c r="J8" s="283"/>
+      <c r="K8" s="283"/>
+      <c r="L8" s="283"/>
+      <c r="M8" s="283"/>
+      <c r="N8" s="283"/>
+      <c r="O8" s="283"/>
+      <c r="P8" s="283"/>
+      <c r="Q8" s="283"/>
+      <c r="R8" s="283"/>
+      <c r="S8" s="283"/>
+      <c r="T8" s="283"/>
+      <c r="U8" s="283"/>
+      <c r="V8" s="283"/>
+      <c r="W8" s="283"/>
+      <c r="X8" s="283"/>
+      <c r="Y8" s="283"/>
+      <c r="Z8" s="283"/>
+      <c r="AA8" s="283"/>
+      <c r="AB8" s="283"/>
+      <c r="AC8" s="283"/>
+      <c r="AD8" s="283"/>
+      <c r="AE8" s="283"/>
+      <c r="AF8" s="283"/>
+      <c r="AG8" s="283"/>
+      <c r="AH8" s="283"/>
+      <c r="AI8" s="283"/>
+      <c r="AJ8" s="283"/>
+      <c r="AK8" s="283"/>
+      <c r="AL8" s="283"/>
+      <c r="AM8" s="283"/>
+      <c r="AN8" s="283"/>
+      <c r="AO8" s="283"/>
+      <c r="AP8" s="283"/>
+      <c r="AQ8" s="283"/>
+      <c r="AR8" s="283"/>
+      <c r="AS8" s="283"/>
+      <c r="AT8" s="283"/>
+      <c r="AU8" s="283"/>
+      <c r="AV8" s="282" t="s">
+        <v>18</v>
+      </c>
+      <c r="AW8" s="282" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="AQ6:AQ8"/>
+    <mergeCell ref="AR6:AR8"/>
+    <mergeCell ref="AS6:AS8"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="AU6:AU8"/>
+    <mergeCell ref="AK6:AK8"/>
+    <mergeCell ref="AL6:AL8"/>
+    <mergeCell ref="AM6:AM8"/>
+    <mergeCell ref="AN6:AN8"/>
+    <mergeCell ref="AO6:AO8"/>
+    <mergeCell ref="AP6:AP8"/>
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="AF6:AF8"/>
+    <mergeCell ref="AG6:AG8"/>
+    <mergeCell ref="AH6:AH8"/>
+    <mergeCell ref="AI6:AI8"/>
+    <mergeCell ref="AJ6:AJ8"/>
+    <mergeCell ref="Y6:Y8"/>
+    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="AA6:AA8"/>
+    <mergeCell ref="AB6:AB8"/>
+    <mergeCell ref="AC6:AC8"/>
+    <mergeCell ref="AD6:AD8"/>
+    <mergeCell ref="S6:S8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="X6:X8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="R6:R8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -12062,10 +12859,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4" collapsed="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="4" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -12091,10 +12888,10 @@
     </row>
     <row r="5" spans="1:9" s="15" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="225" t="s">
         <v>649</v>
       </c>
-      <c r="D5" s="224"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="153"/>
       <c r="F5" s="16"/>
     </row>
@@ -12106,10 +12903,10 @@
       <c r="F6" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="204" t="s">
+      <c r="C8" s="188" t="s">
         <v>653</v>
       </c>
-      <c r="D8" s="206"/>
+      <c r="D8" s="190"/>
       <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -12172,10 +12969,10 @@
     </row>
     <row r="17" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="225" t="s">
+      <c r="C19" s="223" t="s">
         <v>654</v>
       </c>
-      <c r="D19" s="225"/>
+      <c r="D19" s="223"/>
     </row>
     <row r="20" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="39" t="s">
@@ -12228,10 +13025,10 @@
     <row r="27" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="226" t="s">
+      <c r="C29" s="224" t="s">
         <v>655</v>
       </c>
-      <c r="D29" s="226"/>
+      <c r="D29" s="224"/>
     </row>
     <row r="30" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="39" t="s">
@@ -12291,10 +13088,10 @@
     </row>
     <row r="38" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="225" t="s">
+      <c r="C40" s="223" t="s">
         <v>656</v>
       </c>
-      <c r="D40" s="225"/>
+      <c r="D40" s="223"/>
     </row>
     <row r="41" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C41" s="39" t="s">
@@ -12354,10 +13151,10 @@
     </row>
     <row r="49" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C51" s="226" t="s">
+      <c r="C51" s="224" t="s">
         <v>657</v>
       </c>
-      <c r="D51" s="226"/>
+      <c r="D51" s="224"/>
     </row>
     <row r="52" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C52" s="39" t="s">
@@ -12425,10 +13222,10 @@
     </row>
     <row r="61" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C63" s="225" t="s">
+      <c r="C63" s="223" t="s">
         <v>658</v>
       </c>
-      <c r="D63" s="225"/>
+      <c r="D63" s="223"/>
     </row>
     <row r="64" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C64" s="39" t="s">
@@ -12496,10 +13293,10 @@
     </row>
     <row r="73" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C75" s="225" t="s">
+      <c r="C75" s="223" t="s">
         <v>659</v>
       </c>
-      <c r="D75" s="225"/>
+      <c r="D75" s="223"/>
     </row>
     <row r="76" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="39" t="s">
@@ -12559,10 +13356,10 @@
     </row>
     <row r="84" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C86" s="225" t="s">
+      <c r="C86" s="223" t="s">
         <v>660</v>
       </c>
-      <c r="D86" s="225"/>
+      <c r="D86" s="223"/>
     </row>
     <row r="87" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C87" s="39" t="s">
@@ -12622,10 +13419,10 @@
     </row>
     <row r="95" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C97" s="226" t="s">
+      <c r="C97" s="224" t="s">
         <v>661</v>
       </c>
-      <c r="D97" s="226"/>
+      <c r="D97" s="224"/>
     </row>
     <row r="98" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C98" s="39" t="s">
@@ -12693,10 +13490,10 @@
     </row>
     <row r="107" spans="3:4" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C109" s="225" t="s">
+      <c r="C109" s="223" t="s">
         <v>662</v>
       </c>
-      <c r="D109" s="225"/>
+      <c r="D109" s="223"/>
     </row>
     <row r="110" spans="3:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C110" s="39" t="s">
@@ -12757,17 +13554,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C40:D40"/>
     <mergeCell ref="C109:D109"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C40:D40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F1" location="'Rating Algorithm'!A26" display="Rating Algorithm'!A26"/>
@@ -12784,10 +13581,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -12882,9 +13679,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -12905,11 +13702,11 @@
     <row r="5" spans="1:7" s="15" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="153"/>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="225" t="s">
         <v>650</v>
       </c>
       <c r="D5" s="228"/>
-      <c r="E5" s="224"/>
+      <c r="E5" s="226"/>
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -12920,10 +13717,10 @@
       <c r="G6" s="16"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="226" t="s">
+      <c r="C8" s="224" t="s">
         <v>663</v>
       </c>
-      <c r="D8" s="225"/>
+      <c r="D8" s="223"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="39" t="s">
@@ -13114,10 +13911,10 @@
     </row>
     <row r="35" spans="2:9" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C37" s="225" t="s">
+      <c r="C37" s="223" t="s">
         <v>665</v>
       </c>
-      <c r="D37" s="225"/>
+      <c r="D37" s="223"/>
     </row>
     <row r="38" spans="2:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C38" s="39" t="s">
@@ -13188,9 +13985,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -13294,8 +14091,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -13324,11 +14121,11 @@
     <row r="5" spans="1:11" s="15" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="153"/>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="225" t="s">
         <v>651</v>
       </c>
       <c r="D5" s="228"/>
-      <c r="E5" s="224"/>
+      <c r="E5" s="226"/>
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -13377,10 +14174,10 @@
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="226" t="s">
+      <c r="C15" s="224" t="s">
         <v>672</v>
       </c>
-      <c r="D15" s="226"/>
+      <c r="D15" s="224"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="39" t="s">
@@ -13418,10 +14215,10 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="3:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="226" t="s">
+      <c r="C22" s="224" t="s">
         <v>673</v>
       </c>
-      <c r="D22" s="226"/>
+      <c r="D22" s="224"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="3:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -13451,10 +14248,10 @@
     </row>
     <row r="27" spans="3:11" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="226" t="s">
+      <c r="C29" s="224" t="s">
         <v>674</v>
       </c>
-      <c r="D29" s="226"/>
+      <c r="D29" s="224"/>
     </row>
     <row r="30" spans="3:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="39" t="s">
@@ -13482,10 +14279,10 @@
     </row>
     <row r="34" spans="2:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C36" s="226" t="s">
+      <c r="C36" s="224" t="s">
         <v>480</v>
       </c>
-      <c r="D36" s="226"/>
+      <c r="D36" s="224"/>
     </row>
     <row r="37" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="39" t="s">
@@ -13661,9 +14458,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -13828,12 +14625,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15" collapsed="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="15" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -13860,7 +14657,7 @@
     </row>
     <row r="5" spans="1:8" s="15" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
-      <c r="C5" s="188" t="s">
+      <c r="C5" s="214" t="s">
         <v>652</v>
       </c>
       <c r="D5" s="244"/>
@@ -13871,10 +14668,10 @@
       <c r="H6" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="226" t="s">
+      <c r="C8" s="224" t="s">
         <v>675</v>
       </c>
-      <c r="D8" s="226"/>
+      <c r="D8" s="224"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -13934,10 +14731,10 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="226" t="s">
+      <c r="C15" s="224" t="s">
         <v>676</v>
       </c>
-      <c r="D15" s="226"/>
+      <c r="D15" s="224"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
@@ -13997,11 +14794,11 @@
       <c r="H21" s="15"/>
     </row>
     <row r="22" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="204" t="s">
+      <c r="C22" s="188" t="s">
         <v>677</v>
       </c>
-      <c r="D22" s="205"/>
-      <c r="E22" s="206"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="190"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -14047,12 +14844,12 @@
     </row>
     <row r="27" spans="3:8" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="204" t="s">
+      <c r="C29" s="188" t="s">
         <v>678</v>
       </c>
-      <c r="D29" s="205"/>
-      <c r="E29" s="205"/>
-      <c r="F29" s="206"/>
+      <c r="D29" s="189"/>
+      <c r="E29" s="189"/>
+      <c r="F29" s="190"/>
     </row>
     <row r="30" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="39" t="s">

</xml_diff>